<commit_message>
Update a lot of docs for final
</commit_message>
<xml_diff>
--- a/Riskmanagement.xlsx
+++ b/Riskmanagement.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\07 Dokumente\Duales Studium\Nappy-the-ingenious-docs\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035"/>
   </bookViews>
@@ -14,12 +19,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$2:$H$18</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Risk Name</t>
   </si>
@@ -91,12 +96,21 @@
   </si>
   <si>
     <t>Fix issues alone or with help from the others</t>
+  </si>
+  <si>
+    <t>wrong use case implementation</t>
+  </si>
+  <si>
+    <t>the developer misunderstand the requirements</t>
+  </si>
+  <si>
+    <t>Project manager (Ali) will remind you to do the right work! :)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -291,9 +305,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -318,6 +329,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -329,14 +349,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -374,9 +397,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,7 +434,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,7 +469,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -626,12 +649,12 @@
   <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
@@ -660,7 +683,7 @@
       <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -671,20 +694,20 @@
       <c r="C3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="15">
         <v>0.3</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="12">
         <v>9</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="17">
         <f t="shared" ref="F3:F18" si="0">D3*E3</f>
         <v>2.6999999999999997</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -695,17 +718,17 @@
       <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="16">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <v>4</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="12">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="20" t="s">
         <v>16</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -719,17 +742,17 @@
       <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="16">
         <v>0.7</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <v>3</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="12">
         <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="20" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -743,17 +766,17 @@
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="16">
         <v>0.75</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="13">
         <v>2</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="12">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="20" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -767,153 +790,165 @@
       <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="16">
         <v>0.9</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>1</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="12">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="3"/>
+    <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="13">
+        <v>4</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="11"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="20"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="20"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="11"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="20"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="11"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="20"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="11"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="20"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="11"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="20"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="11"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="20"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="11"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="20"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="11"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="20"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="12"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="21"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated Riskmanagement: added flapping tests
</commit_message>
<xml_diff>
--- a/Riskmanagement.xlsx
+++ b/Riskmanagement.xlsx
@@ -15,13 +15,14 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Tabelle1!$B$2:$H$18</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Tabelle1!$B$2:$H$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Tabelle1!$B$2:$H$18</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Risk Name</t>
   </si>
@@ -74,7 +75,7 @@
     <t>Use cases are to big to get implemented</t>
   </si>
   <si>
-    <t>Split into smaller use cases or abort. </t>
+    <t>Split into smaller use cases or abort.</t>
   </si>
   <si>
     <t>loss of knowledge</t>
@@ -84,6 +85,15 @@
   </si>
   <si>
     <t>relearn and new planning</t>
+  </si>
+  <si>
+    <t>Flapping Tests</t>
+  </si>
+  <si>
+    <t>Tests which randomly work and fail</t>
+  </si>
+  <si>
+    <t>Repair Test</t>
   </si>
   <si>
     <t>technical issues</t>
@@ -383,7 +393,7 @@
   <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -527,14 +537,14 @@
         <v>22</v>
       </c>
       <c r="D7" s="13" t="n">
-        <v>0.9</v>
+        <v>0.25</v>
       </c>
       <c r="E7" s="14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" s="7" t="n">
         <f aca="false">D7*E7</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>23</v>
@@ -551,20 +561,20 @@
         <v>25</v>
       </c>
       <c r="D8" s="13" t="n">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="E8" s="14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7" t="n">
         <f aca="false">D8*E8</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,23 +585,23 @@
         <v>28</v>
       </c>
       <c r="D9" s="13" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E9" s="14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F9" s="7" t="n">
         <f aca="false">D9*E9</f>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>29</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="11" t="s">
         <v>30</v>
       </c>
@@ -599,14 +609,14 @@
         <v>31</v>
       </c>
       <c r="D10" s="13" t="n">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E10" s="14" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F10" s="7" t="n">
         <f aca="false">D10*E10</f>
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>32</v>
@@ -615,22 +625,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+    <row r="11" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="13" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="14" t="n">
+        <v>7</v>
+      </c>
       <c r="F11" s="7" t="n">
         <f aca="false">D11*E11</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="11"/>
+        <v>0.35</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="14"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="7" t="n">
         <f aca="false">D12*E12</f>

</xml_diff>